<commit_message>
Cambios en planilla Excel
</commit_message>
<xml_diff>
--- a/Otros/ingreasar no conformidad.xlsx
+++ b/Otros/ingreasar no conformidad.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MIGUEL AIEP\3 Tercer Año\6° Semestre\Taller Avanzado de Programación de Análisis\CSNC\trunk\Otros\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SVN\SCSNC\trunk\Otros\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>no conformidad</t>
   </si>
@@ -35,27 +35,6 @@
     <t>no conformidad Capacitacion</t>
   </si>
   <si>
-    <t>falla en el cumplimiento de las especificaciones de una actividad de capacitacion</t>
-  </si>
-  <si>
-    <t>falla en el cumplimiento de disponer la infraestructura y equipos necesarios</t>
-  </si>
-  <si>
-    <t>materiales de servicios de capacitacion inadecuados</t>
-  </si>
-  <si>
-    <t>falla en el cumplimiento de las exigencias de seguridad y salud ocupacional</t>
-  </si>
-  <si>
-    <t>deficiencias en el sistema de gestion de la calidad del organismo de capacitacion</t>
-  </si>
-  <si>
-    <t>instrumentos de capacitacion inadecuados</t>
-  </si>
-  <si>
-    <t>relatores y/o facilitadores no son evaluados  en terminos de desempeño, dentro de las espectativas del organsmo</t>
-  </si>
-  <si>
     <t>ingresar no conformidad</t>
   </si>
   <si>
@@ -75,6 +54,36 @@
   </si>
   <si>
     <t>reclamo de relatores o facilitadores</t>
+  </si>
+  <si>
+    <t>', 1)</t>
+  </si>
+  <si>
+    <t>('</t>
+  </si>
+  <si>
+    <t>', 1) ,</t>
+  </si>
+  <si>
+    <t>Falla en el cumplimiento de las especificaciones de una actividad de capacitacion</t>
+  </si>
+  <si>
+    <t>Falla en el cumplimiento de disponer la infraestructura y equipos necesarios</t>
+  </si>
+  <si>
+    <t>Materiales de servicios de capacitacion inadecuados</t>
+  </si>
+  <si>
+    <t>Falla en el cumplimiento de las exigencias de seguridad y salud ocupacional</t>
+  </si>
+  <si>
+    <t>Deficiencias en el sistema de gestion de la calidad del organismo de capacitacion</t>
+  </si>
+  <si>
+    <t>Instrumentos de capacitacion inadecuados</t>
+  </si>
+  <si>
+    <t>Relatores y/o facilitadores no son evaluados  en terminos de desempeño, dentro de las espectativas del organsmo</t>
   </si>
 </sst>
 </file>
@@ -110,8 +119,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,99 +402,144 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.7109375" customWidth="1"/>
-    <col min="2" max="2" width="102.5703125" customWidth="1"/>
+    <col min="2" max="2" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="102.5703125" customWidth="1"/>
+    <col min="4" max="4" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se actualiza el modelo de datos y se estructura el documento Excel para el ingreso y generación de script SQL
</commit_message>
<xml_diff>
--- a/Otros/ingreasar no conformidad.xlsx
+++ b/Otros/ingreasar no conformidad.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="DropDownLists" sheetId="1" r:id="rId1"/>
+    <sheet name="UrlAccess" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,19 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
-  <si>
-    <t>no conformidad</t>
-  </si>
-  <si>
-    <t>no conformidad potencial</t>
-  </si>
-  <si>
-    <t>no conformidad Capacitacion</t>
-  </si>
-  <si>
-    <t>ingresar no conformidad</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
     <t>TIPO DE INCIDENCIA</t>
   </si>
@@ -50,21 +39,6 @@
     <t>Reclamo de cliente</t>
   </si>
   <si>
-    <t>reclamo de proveedores</t>
-  </si>
-  <si>
-    <t>reclamo de relatores o facilitadores</t>
-  </si>
-  <si>
-    <t>', 1)</t>
-  </si>
-  <si>
-    <t>('</t>
-  </si>
-  <si>
-    <t>', 1) ,</t>
-  </si>
-  <si>
     <t>Falla en el cumplimiento de las especificaciones de una actividad de capacitacion</t>
   </si>
   <si>
@@ -84,6 +58,66 @@
   </si>
   <si>
     <t>Relatores y/o facilitadores no son evaluados  en terminos de desempeño, dentro de las espectativas del organsmo</t>
+  </si>
+  <si>
+    <t>Reclamo de proveedores</t>
+  </si>
+  <si>
+    <t>Reclamo de relatores o facilitadores</t>
+  </si>
+  <si>
+    <t>TiposIncidencias</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Descripción</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>ModosDeteccion</t>
+  </si>
+  <si>
+    <t>Entidad</t>
+  </si>
+  <si>
+    <t>Tabla</t>
+  </si>
+  <si>
+    <t>Script SQL</t>
+  </si>
+  <si>
+    <t>ESTADOS INCIDENCIAS</t>
+  </si>
+  <si>
+    <t>TRATAMIENTOS</t>
+  </si>
+  <si>
+    <t>ACCIONES</t>
+  </si>
+  <si>
+    <t>ROLES</t>
+  </si>
+  <si>
+    <t>Acceso</t>
+  </si>
+  <si>
+    <t>Url de acceso</t>
+  </si>
+  <si>
+    <t>:</t>
+  </si>
+  <si>
+    <t>Accesos</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>/Test.aspx</t>
   </si>
 </sst>
 </file>
@@ -107,7 +141,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -115,13 +149,57 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,148 +480,340 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" customWidth="1"/>
-    <col min="2" max="2" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="102.5703125" customWidth="1"/>
-    <col min="4" max="4" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.7109375" customWidth="1"/>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="102.5703125" customWidth="1"/>
+    <col min="5" max="5" width="4" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" customWidth="1"/>
+    <col min="7" max="7" width="145.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" t="str">
+        <f>CONCATENATE("INSERT INTO ",B3," VALUES (",C3,", '",D3,"', ",IF(E3=1,1,0),")")</f>
+        <v>INSERT INTO TiposIncidencias VALUES (1, 'Falla en el cumplimiento de las especificaciones de una actividad de capacitacion', 1)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" ref="G4:G14" si="0">CONCATENATE("INSERT INTO ",B4," VALUES (",C4,", '",D4,"', ",IF(E4=1,1,0),")")</f>
+        <v>INSERT INTO TiposIncidencias VALUES (2, 'Falla en el cumplimiento de disponer la infraestructura y equipos necesarios', 1)</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO TiposIncidencias VALUES (3, 'Materiales de servicios de capacitacion inadecuados', 1)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO TiposIncidencias VALUES (4, 'Falla en el cumplimiento de las exigencias de seguridad y salud ocupacional', 1)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO TiposIncidencias VALUES (5, 'Deficiencias en el sistema de gestion de la calidad del organismo de capacitacion', 1)</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="1">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO TiposIncidencias VALUES (6, 'Instrumentos de capacitacion inadecuados', 1)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO TiposIncidencias VALUES (7, 'Relatores y/o facilitadores no son evaluados  en terminos de desempeño, dentro de las espectativas del organsmo', 1)</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ModosDeteccion VALUES (1, 'Auditoria interna', 1)</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ModosDeteccion VALUES (2, 'Reclamo de cliente', 1)</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="1">
+        <v>3</v>
+      </c>
+      <c r="D13" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ModosDeteccion VALUES (3, 'Reclamo de proveedores', 1)</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="1">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ModosDeteccion VALUES (4, 'Reclamo de relatores o facilitadores', 1)</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>9</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" customWidth="1"/>
+    <col min="4" max="4" width="33.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7" customWidth="1"/>
+    <col min="6" max="6" width="57.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" t="str">
+        <f>CONCATENATE("INSERT INTO ",$C$1," VALUES (",B5,", '",C5,"', '",D5,"')")</f>
+        <v>INSERT INTO Accesos VALUES (1, 'Test', '/Test.aspx')</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se rellenan las tablas restantes, se añade tabla regiones, provinicas, y regiones, en proceso de actualización
</commit_message>
<xml_diff>
--- a/Otros/ingreasar no conformidad.xlsx
+++ b/Otros/ingreasar no conformidad.xlsx
@@ -1,21 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SVN\SCSNC\trunk\Otros\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="DropDownLists" sheetId="1" r:id="rId1"/>
     <sheet name="UrlAccess" sheetId="2" r:id="rId2"/>
+    <sheet name="Regiones  Provincias Comunas" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="120">
   <si>
     <t>TIPO DE INCIDENCIA</t>
   </si>
@@ -96,9 +92,6 @@
     <t>TRATAMIENTOS</t>
   </si>
   <si>
-    <t>ACCIONES</t>
-  </si>
-  <si>
     <t>ROLES</t>
   </si>
   <si>
@@ -114,10 +107,280 @@
     <t>Accesos</t>
   </si>
   <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>/Test.aspx</t>
+    <t>EstadosIncidencia</t>
+  </si>
+  <si>
+    <t>Rechazada</t>
+  </si>
+  <si>
+    <t>Revisón de Cumplimiento</t>
+  </si>
+  <si>
+    <t>Análisis de Causas</t>
+  </si>
+  <si>
+    <t>Es espera de revisión</t>
+  </si>
+  <si>
+    <t>Re-Análisis</t>
+  </si>
+  <si>
+    <t>Tratamientos</t>
+  </si>
+  <si>
+    <t>Concesión</t>
+  </si>
+  <si>
+    <t>Desecho</t>
+  </si>
+  <si>
+    <t>Finalizada</t>
+  </si>
+  <si>
+    <t>Liberar</t>
+  </si>
+  <si>
+    <t>Permiso de Desviación</t>
+  </si>
+  <si>
+    <t>Reclasificación</t>
+  </si>
+  <si>
+    <t>Reparación</t>
+  </si>
+  <si>
+    <t>Reproceso</t>
+  </si>
+  <si>
+    <t>Verificación</t>
+  </si>
+  <si>
+    <t>Director Responsable</t>
+  </si>
+  <si>
+    <t>Roles</t>
+  </si>
+  <si>
+    <t>Coordinador</t>
+  </si>
+  <si>
+    <t>Representante Alta Dirección</t>
+  </si>
+  <si>
+    <t>Agregar Usuario</t>
+  </si>
+  <si>
+    <t>/AgregarUsuario.aspx</t>
+  </si>
+  <si>
+    <t>Ingresar No Conformidad</t>
+  </si>
+  <si>
+    <t>/IngresarNoConformidad.aspx</t>
+  </si>
+  <si>
+    <t>/AnalizarNoConformidad.aspx</t>
+  </si>
+  <si>
+    <t>Analizar No Conformidad</t>
+  </si>
+  <si>
+    <t>Gestión de Incidencias</t>
+  </si>
+  <si>
+    <t>/GestionIncidencias.aspx</t>
+  </si>
+  <si>
+    <t>Menú Principal</t>
+  </si>
+  <si>
+    <t>/MainModulos.aspx</t>
+  </si>
+  <si>
+    <t>Revisión de Cumplimiento</t>
+  </si>
+  <si>
+    <t>/RevisionCumplimiento.aspx</t>
+  </si>
+  <si>
+    <t>REGIONES</t>
+  </si>
+  <si>
+    <t>Regiones</t>
+  </si>
+  <si>
+    <t>XV de Arica y Parinacota</t>
+  </si>
+  <si>
+    <t>I de Tarapacá</t>
+  </si>
+  <si>
+    <t>II de Antofagasta</t>
+  </si>
+  <si>
+    <t>III de Atacama</t>
+  </si>
+  <si>
+    <t>IV de Coquimbo</t>
+  </si>
+  <si>
+    <t>V de Valparaíso</t>
+  </si>
+  <si>
+    <t>VI del Libertador General Bernardo O'Higgins</t>
+  </si>
+  <si>
+    <t>VII del Maule</t>
+  </si>
+  <si>
+    <t>VIII del Bío Bío</t>
+  </si>
+  <si>
+    <t>IX de la Araucanía</t>
+  </si>
+  <si>
+    <t>XIV de los Ríos</t>
+  </si>
+  <si>
+    <t>X de los Lagos</t>
+  </si>
+  <si>
+    <t>XI Aisén del General Carlos Ibáñez del Campo</t>
+  </si>
+  <si>
+    <t>XII de Magallanes y Antártica Chilena</t>
+  </si>
+  <si>
+    <t>Metropolitana de Santiago</t>
+  </si>
+  <si>
+    <t>PROVINCIAS</t>
+  </si>
+  <si>
+    <t>Provincia de Arica</t>
+  </si>
+  <si>
+    <t>Provincia de Parinacota</t>
+  </si>
+  <si>
+    <t>COMUNAS</t>
+  </si>
+  <si>
+    <t>Comunas</t>
+  </si>
+  <si>
+    <t>Provincias</t>
+  </si>
+  <si>
+    <t>Putre</t>
+  </si>
+  <si>
+    <t>Arica</t>
+  </si>
+  <si>
+    <t>Camarones</t>
+  </si>
+  <si>
+    <t>General Lagos</t>
+  </si>
+  <si>
+    <t>Provincia de Iquique</t>
+  </si>
+  <si>
+    <t>Alto Hospicio</t>
+  </si>
+  <si>
+    <t>Iquique</t>
+  </si>
+  <si>
+    <t>Provincia Del Tamarugal</t>
+  </si>
+  <si>
+    <t>Huara</t>
+  </si>
+  <si>
+    <t>Camiña</t>
+  </si>
+  <si>
+    <t>Colchane</t>
+  </si>
+  <si>
+    <t>Pica</t>
+  </si>
+  <si>
+    <t>Pozo Almonte</t>
+  </si>
+  <si>
+    <t>Provincia de Tocopilla</t>
+  </si>
+  <si>
+    <t>Tocopilla</t>
+  </si>
+  <si>
+    <t>María Elena</t>
+  </si>
+  <si>
+    <t>Provincia de El Loa</t>
+  </si>
+  <si>
+    <t>Calama</t>
+  </si>
+  <si>
+    <t>Ollagüe</t>
+  </si>
+  <si>
+    <t>San Pedro de Atacama</t>
+  </si>
+  <si>
+    <t>Provincia de Antofagasta</t>
+  </si>
+  <si>
+    <t>Antofagasta</t>
+  </si>
+  <si>
+    <t>Mejillones</t>
+  </si>
+  <si>
+    <t>Sierra Gorda</t>
+  </si>
+  <si>
+    <t>Taltal</t>
+  </si>
+  <si>
+    <t>Provincia de Chañaral</t>
+  </si>
+  <si>
+    <t>Chañaral</t>
+  </si>
+  <si>
+    <t>Diego de Almagro</t>
+  </si>
+  <si>
+    <t>Provincia de Copiapó</t>
+  </si>
+  <si>
+    <t>Copiapó</t>
+  </si>
+  <si>
+    <t>Caldera</t>
+  </si>
+  <si>
+    <t>Tierra Amarilla</t>
+  </si>
+  <si>
+    <t>Provincia de Huasco</t>
+  </si>
+  <si>
+    <t>Vallenar</t>
+  </si>
+  <si>
+    <t>Freirina</t>
+  </si>
+  <si>
+    <t>Huasco</t>
+  </si>
+  <si>
+    <t>Alto del Carmen</t>
   </si>
 </sst>
 </file>
@@ -260,7 +523,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -295,7 +558,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -472,7 +735,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -480,10 +743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D50" sqref="A36:D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,7 +755,7 @@
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="2.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="102.5703125" customWidth="1"/>
-    <col min="5" max="5" width="4" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.85546875" customWidth="1"/>
     <col min="7" max="7" width="145.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -725,20 +988,483 @@
       <c r="A16" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="str">
+        <f>CONCATENATE("INSERT INTO ",B16," VALUES (",C16,", '",D16,"', ",IF(E16=1,1,0),")")</f>
+        <v>INSERT INTO EstadosIncidencia VALUES (1, 'Análisis de Causas', 1)</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" ref="G17:G21" si="1">CONCATENATE("INSERT INTO ",B17," VALUES (",C17,", '",D17,"', ",IF(E17=1,1,0),")")</f>
+        <v>INSERT INTO EstadosIncidencia VALUES (2, 'Rechazada', 1)</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO EstadosIncidencia VALUES (3, 'Es espera de revisión', 1)</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO EstadosIncidencia VALUES (4, 'Revisón de Cumplimiento', 1)</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO EstadosIncidencia VALUES (5, 'Re-Análisis', 1)</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO EstadosIncidencia VALUES (6, 'Finalizada', 1)</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="G23" t="str">
+        <f>CONCATENATE("INSERT INTO ",B23," VALUES (",C23,", '",D23,"', ",IF(E23=1,1,0),")")</f>
+        <v>INSERT INTO Tratamientos VALUES (1, 'Concesión', 1)</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" ref="G24:G34" si="2">CONCATENATE("INSERT INTO ",B24," VALUES (",C24,", '",D24,"', ",IF(E24=1,1,0),")")</f>
+        <v>INSERT INTO Tratamientos VALUES (2, 'Desecho', 1)</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO Tratamientos VALUES (3, 'Liberar', 1)</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO Tratamientos VALUES (4, 'Permiso de Desviación', 1)</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27">
+        <v>5</v>
+      </c>
+      <c r="D27" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO Tratamientos VALUES (5, 'Reclasificación', 1)</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28">
+        <v>6</v>
+      </c>
+      <c r="D28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO Tratamientos VALUES (6, 'Reparación', 1)</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29">
+        <v>7</v>
+      </c>
+      <c r="D29" t="s">
+        <v>42</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO Tratamientos VALUES (7, 'Reproceso', 1)</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30">
+        <v>8</v>
+      </c>
+      <c r="D30" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO Tratamientos VALUES (8, 'Verificación', 1)</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>24</v>
+      <c r="B32" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>46</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO Roles VALUES (1, 'Coordinador', 1)</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>44</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO Roles VALUES (2, 'Director Responsable', 1)</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34">
+        <v>3</v>
+      </c>
+      <c r="D34" t="s">
+        <v>47</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO Roles VALUES (3, 'Representante Alta Dirección', 1)</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>61</v>
+      </c>
+      <c r="C38">
+        <v>3</v>
+      </c>
+      <c r="D38" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>61</v>
+      </c>
+      <c r="C39">
+        <v>4</v>
+      </c>
+      <c r="D39" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40">
+        <v>5</v>
+      </c>
+      <c r="D40" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>61</v>
+      </c>
+      <c r="C41">
+        <v>6</v>
+      </c>
+      <c r="D41" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>61</v>
+      </c>
+      <c r="C42">
+        <v>7</v>
+      </c>
+      <c r="D42" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43">
+        <v>8</v>
+      </c>
+      <c r="D43" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>61</v>
+      </c>
+      <c r="C44">
+        <v>9</v>
+      </c>
+      <c r="D44" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>61</v>
+      </c>
+      <c r="C45">
+        <v>10</v>
+      </c>
+      <c r="D45" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>61</v>
+      </c>
+      <c r="C46">
+        <v>11</v>
+      </c>
+      <c r="D46" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>61</v>
+      </c>
+      <c r="C47">
+        <v>12</v>
+      </c>
+      <c r="D47" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>61</v>
+      </c>
+      <c r="C48">
+        <v>13</v>
+      </c>
+      <c r="D48" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>61</v>
+      </c>
+      <c r="C49">
+        <v>14</v>
+      </c>
+      <c r="D49" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>61</v>
+      </c>
+      <c r="C50">
+        <v>15</v>
+      </c>
+      <c r="D50" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -749,10 +1475,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,7 +1488,7 @@
     <col min="3" max="3" width="30.5703125" customWidth="1"/>
     <col min="4" max="4" width="33.7109375" customWidth="1"/>
     <col min="5" max="5" width="7" customWidth="1"/>
-    <col min="6" max="6" width="57.28515625" customWidth="1"/>
+    <col min="6" max="6" width="84.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -770,15 +1496,15 @@
         <v>19</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
@@ -787,7 +1513,7 @@
         <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
@@ -798,19 +1524,932 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="F5" t="str">
         <f>CONCATENATE("INSERT INTO ",$C$1," VALUES (",B5,", '",C5,"', '",D5,"')")</f>
-        <v>INSERT INTO Accesos VALUES (1, 'Test', '/Test.aspx')</v>
+        <v>INSERT INTO Accesos VALUES (1, 'Agregar Usuario', '/AgregarUsuario.aspx')</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" t="str">
+        <f>CONCATENATE("INSERT INTO ",$C$1," VALUES (",B6,", '",C6,"', '",D6,"')")</f>
+        <v>INSERT INTO Accesos VALUES (2, 'Ingresar No Conformidad', '/IngresarNoConformidad.aspx')</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" t="str">
+        <f>CONCATENATE("INSERT INTO ",$C$1," VALUES (",B7,", '",C7,"', '",D7,"')")</f>
+        <v>INSERT INTO Accesos VALUES (3, 'Analizar No Conformidad', '/AnalizarNoConformidad.aspx')</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" t="str">
+        <f>CONCATENATE("INSERT INTO ",$C$1," VALUES (",B8,", '",C8,"', '",D8,"')")</f>
+        <v>INSERT INTO Accesos VALUES (4, 'Gestión de Incidencias', '/GestionIncidencias.aspx')</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" t="str">
+        <f>CONCATENATE("INSERT INTO ",$C$1," VALUES (",B9,", '",C9,"', '",D9,"')")</f>
+        <v>INSERT INTO Accesos VALUES (5, 'Menú Principal', '/MainModulos.aspx')</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" t="str">
+        <f>CONCATENATE("INSERT INTO ",$C$1," VALUES (",B10,", '",C10,"', '",D10,"')")</f>
+        <v>INSERT INTO Accesos VALUES (6, 'Revisión de Cumplimiento', '/RevisionCumplimiento.aspx')</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:O93"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>78</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>80</v>
+      </c>
+      <c r="M3" t="s">
+        <v>81</v>
+      </c>
+      <c r="N3" t="s">
+        <v>84</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>63</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4" t="s">
+        <v>79</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="N4" t="s">
+        <v>85</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5" t="s">
+        <v>87</v>
+      </c>
+      <c r="N5" t="s">
+        <v>83</v>
+      </c>
+      <c r="O5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6" t="s">
+        <v>90</v>
+      </c>
+      <c r="N6" t="s">
+        <v>86</v>
+      </c>
+      <c r="O6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7" t="s">
+        <v>96</v>
+      </c>
+      <c r="N7" t="s">
+        <v>88</v>
+      </c>
+      <c r="O7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8">
+        <v>6</v>
+      </c>
+      <c r="I8" t="s">
+        <v>99</v>
+      </c>
+      <c r="N8" t="s">
+        <v>89</v>
+      </c>
+      <c r="O8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9">
+        <v>7</v>
+      </c>
+      <c r="I9" t="s">
+        <v>103</v>
+      </c>
+      <c r="N9" t="s">
+        <v>91</v>
+      </c>
+      <c r="O9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10">
+        <v>8</v>
+      </c>
+      <c r="I10" t="s">
+        <v>108</v>
+      </c>
+      <c r="N10" t="s">
+        <v>92</v>
+      </c>
+      <c r="O10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>70</v>
+      </c>
+      <c r="H11">
+        <v>9</v>
+      </c>
+      <c r="I11" t="s">
+        <v>111</v>
+      </c>
+      <c r="N11" t="s">
+        <v>93</v>
+      </c>
+      <c r="O11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>71</v>
+      </c>
+      <c r="H12">
+        <v>10</v>
+      </c>
+      <c r="I12" t="s">
+        <v>115</v>
+      </c>
+      <c r="N12" t="s">
+        <v>94</v>
+      </c>
+      <c r="O12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>72</v>
+      </c>
+      <c r="H13">
+        <v>11</v>
+      </c>
+      <c r="N13" t="s">
+        <v>95</v>
+      </c>
+      <c r="O13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>73</v>
+      </c>
+      <c r="H14">
+        <v>12</v>
+      </c>
+      <c r="N14" t="s">
+        <v>97</v>
+      </c>
+      <c r="O14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>74</v>
+      </c>
+      <c r="H15">
+        <v>13</v>
+      </c>
+      <c r="N15" t="s">
+        <v>98</v>
+      </c>
+      <c r="O15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16">
+        <v>14</v>
+      </c>
+      <c r="D16" t="s">
+        <v>75</v>
+      </c>
+      <c r="H16">
+        <v>14</v>
+      </c>
+      <c r="N16" t="s">
+        <v>100</v>
+      </c>
+      <c r="O16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17">
+        <v>15</v>
+      </c>
+      <c r="D17" t="s">
+        <v>76</v>
+      </c>
+      <c r="H17">
+        <v>15</v>
+      </c>
+      <c r="N17" t="s">
+        <v>101</v>
+      </c>
+      <c r="O17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <v>16</v>
+      </c>
+      <c r="N18" t="s">
+        <v>102</v>
+      </c>
+      <c r="O18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H19">
+        <v>17</v>
+      </c>
+      <c r="N19" t="s">
+        <v>104</v>
+      </c>
+      <c r="O19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <v>18</v>
+      </c>
+      <c r="N20" t="s">
+        <v>105</v>
+      </c>
+      <c r="O20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H21">
+        <v>19</v>
+      </c>
+      <c r="N21" t="s">
+        <v>106</v>
+      </c>
+      <c r="O21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H22">
+        <v>20</v>
+      </c>
+      <c r="N22" t="s">
+        <v>107</v>
+      </c>
+      <c r="O22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <v>21</v>
+      </c>
+      <c r="N23" t="s">
+        <v>109</v>
+      </c>
+      <c r="O23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H24">
+        <v>22</v>
+      </c>
+      <c r="N24" t="s">
+        <v>110</v>
+      </c>
+      <c r="O24">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H25">
+        <v>23</v>
+      </c>
+      <c r="N25" t="s">
+        <v>112</v>
+      </c>
+      <c r="O25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H26">
+        <v>24</v>
+      </c>
+      <c r="N26" t="s">
+        <v>113</v>
+      </c>
+      <c r="O26">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H27">
+        <v>25</v>
+      </c>
+      <c r="N27" t="s">
+        <v>114</v>
+      </c>
+      <c r="O27">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H28">
+        <v>26</v>
+      </c>
+      <c r="N28" t="s">
+        <v>116</v>
+      </c>
+      <c r="O28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H29">
+        <v>27</v>
+      </c>
+      <c r="N29" t="s">
+        <v>117</v>
+      </c>
+      <c r="O29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H30">
+        <v>28</v>
+      </c>
+      <c r="N30" t="s">
+        <v>118</v>
+      </c>
+      <c r="O30">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H31">
+        <v>29</v>
+      </c>
+      <c r="N31" t="s">
+        <v>119</v>
+      </c>
+      <c r="O31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H32">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H33">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H34">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H36">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H37">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H38">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H39">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H40">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H41">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H42">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H43">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H44">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H45">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H46">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H47">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H48">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H49">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H50">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H51">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H52">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H53">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H54">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H55">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H56">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H57">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H58">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H59">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H60">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H61">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H62">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H63">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H64">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H65">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H66">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H67">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H68">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H69">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H70">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H71">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H72">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H73">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H74">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H75">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H76">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H77">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H78">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="79" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H79">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="80" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H80">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="81" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H81">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="82" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H82">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="83" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H83">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="84" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H84">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="85" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H85">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="86" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H86">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="87" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H87">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="88" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H88">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="89" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H89">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="90" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H90">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="91" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H91">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="92" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H92">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="93" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H93">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>